<commit_message>
added post condition set and block
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="19035" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="19035" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="794">
   <si>
     <t>Ever Tested?</t>
   </si>
@@ -3094,6 +3094,9 @@
   </si>
   <si>
     <t>25ed04e-852f-11e7-bb31-be2e44b06b34</t>
+  </si>
+  <si>
+    <t>Allow</t>
   </si>
 </sst>
 </file>
@@ -3652,6 +3655,9 @@
     <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3663,9 +3669,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3987,7 +3990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A15"/>
     </sheetView>
   </sheetViews>
@@ -5039,7 +5042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -5991,7 +5994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -6030,34 +6033,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="53"/>
       <c r="D1" s="21"/>
       <c r="G1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="83"/>
+      <c r="J1" s="84"/>
       <c r="K1" s="21"/>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="N1" s="85"/>
-      <c r="T1" s="83" t="s">
+      <c r="N1" s="86"/>
+      <c r="T1" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="21"/>
-      <c r="Y1" s="86" t="s">
+      <c r="Y1" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="Z1" s="86"/>
+      <c r="Z1" s="87"/>
       <c r="AC1" t="s">
         <v>681</v>
       </c>
@@ -9034,8 +9037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="75.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9158,7 +9161,7 @@
         <v>474</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>777</v>
+        <v>700</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>763</v>
@@ -9167,22 +9170,20 @@
         <v>764</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>718</v>
+        <v>654</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="58" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="58" t="s">
-        <v>718</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K4" s="3"/>
       <c r="L4" s="3">
         <v>0</v>
       </c>
@@ -9209,12 +9210,14 @@
         <v>747</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J5" s="3">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="58" t="s">
+        <v>718</v>
+      </c>
       <c r="L5" s="3">
         <v>0</v>
       </c>
@@ -9224,27 +9227,29 @@
         <v>476</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="3" t="s">
-        <v>784</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>718</v>
+      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="58"/>
+      <c r="H6" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>653</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3">
         <v>0</v>
       </c>
@@ -9254,27 +9259,29 @@
         <v>477</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="3" t="s">
-        <v>785</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>719</v>
+      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="58"/>
+      <c r="H7" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="I7" s="3" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>654</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3">
         <v>0</v>
       </c>
@@ -9297,12 +9304,14 @@
       <c r="G8" s="3"/>
       <c r="H8" s="58"/>
       <c r="I8" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J8" s="3">
-        <v>2</v>
-      </c>
-      <c r="K8" s="58"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="58" t="s">
+        <v>653</v>
+      </c>
       <c r="L8" s="3">
         <v>0</v>
       </c>
@@ -9325,12 +9334,14 @@
       <c r="G9" s="3"/>
       <c r="H9" s="58"/>
       <c r="I9" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J9" s="3">
-        <v>2</v>
-      </c>
-      <c r="K9" s="58"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>654</v>
+      </c>
       <c r="L9" s="3">
         <v>0</v>
       </c>
@@ -9339,19 +9350,57 @@
       <c r="A10" t="s">
         <v>480</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="58" t="s">
+        <v>700</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="58"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
       <c r="K10" s="58"/>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>481</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="58" t="s">
+        <v>700</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" s="58"/>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -9412,13 +9461,13 @@
           <x14:formula1>
             <xm:f>Configs!$O$3:$O$33</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K4 K6:K10 E2:E9</xm:sqref>
+          <xm:sqref>K3 K8:K11 K5 E8:E11 E2:E7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>HTS!$H$2:$H$25</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H10 B2:B10</xm:sqref>
+          <xm:sqref>H2:H7 B8:B11 B2:B7 H8:H11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9452,46 +9501,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="83" t="s">
         <v>755</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="83" t="s">
         <v>787</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="83" t="s">
         <v>788</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="83" t="s">
         <v>789</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="83" t="s">
         <v>757</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="83" t="s">
         <v>758</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="83" t="s">
         <v>759</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="83" t="s">
         <v>760</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="83" t="s">
         <v>761</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="K1" s="83" t="s">
         <v>773</v>
       </c>
-      <c r="L1" s="87" t="s">
+      <c r="L1" s="83" t="s">
         <v>783</v>
       </c>
-      <c r="M1" s="87" t="s">
+      <c r="M1" s="83" t="s">
         <v>693</v>
       </c>
-      <c r="N1" s="87" t="s">
+      <c r="N1" s="83" t="s">
         <v>694</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed pre transformations for complex operations
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="794">
   <si>
     <t>Ever Tested?</t>
   </si>
@@ -9035,10 +9035,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="75.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9057,7 +9057,7 @@
     <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
         <v>103</v>
       </c>
@@ -9095,36 +9095,39 @@
         <v>694</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>472</v>
       </c>
       <c r="B2" s="58" t="s">
         <v>700</v>
       </c>
-      <c r="C2" t="s">
-        <v>763</v>
-      </c>
-      <c r="D2" t="s">
-        <v>764</v>
-      </c>
-      <c r="E2" s="58" t="s">
+      <c r="C2" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="58" t="s">
+        <v>700</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="58" t="s">
         <v>653</v>
       </c>
-      <c r="H2" s="58" t="s">
-        <v>749</v>
-      </c>
-      <c r="I2" t="s">
-        <v>776</v>
-      </c>
-      <c r="J2" s="3">
-        <v>2</v>
-      </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>473</v>
       </c>
@@ -9132,13 +9135,11 @@
         <v>700</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>653</v>
+        <v>774</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="3" t="s">
+        <v>784</v>
       </c>
       <c r="H3" s="58" t="s">
         <v>749</v>
@@ -9147,7 +9148,7 @@
         <v>775</v>
       </c>
       <c r="J3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="58" t="s">
         <v>647</v>
@@ -9156,7 +9157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>474</v>
       </c>
@@ -9164,129 +9165,122 @@
         <v>700</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>774</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="3" t="s">
+        <v>784</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="58" t="s">
         <v>749</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
       <c r="J4" s="3">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="K4" s="58"/>
       <c r="L4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>475</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>777</v>
+        <v>700</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>718</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>774</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="3" t="s">
+        <v>784</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="58" t="s">
-        <v>747</v>
+        <v>700</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="58" t="s">
-        <v>718</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K5" s="58"/>
       <c r="L5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>476</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>777</v>
+        <v>700</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>718</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>774</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="3" t="s">
+        <v>785</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="58" t="s">
-        <v>747</v>
+        <v>700</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J6" s="3">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="58" t="s">
+        <v>654</v>
+      </c>
       <c r="L6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>477</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>777</v>
+        <v>700</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>764</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>719</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>774</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="3" t="s">
+        <v>785</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="58" t="s">
-        <v>747</v>
+        <v>700</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
       <c r="J7" s="3">
-        <v>3</v>
-      </c>
-      <c r="K7" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="K7" s="58"/>
       <c r="L7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>478</v>
       </c>
@@ -9299,40 +9293,44 @@
       <c r="D8" s="3"/>
       <c r="E8" s="58"/>
       <c r="F8" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="58"/>
+      <c r="H8" s="58" t="s">
+        <v>749</v>
+      </c>
       <c r="I8" s="3" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="58" t="s">
-        <v>653</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K8" s="58"/>
       <c r="L8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>479</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="3" t="s">
-        <v>785</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>718</v>
+      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="58"/>
+      <c r="H9" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="I9" s="3" t="s">
         <v>775</v>
       </c>
@@ -9340,89 +9338,97 @@
         <v>1</v>
       </c>
       <c r="K9" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="L9" s="3">
+        <v>718</v>
+      </c>
+      <c r="L9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>480</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="3" t="s">
-        <v>784</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>718</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="58"/>
+      <c r="H10" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="I10" s="3" t="s">
         <v>776</v>
       </c>
       <c r="J10" s="3">
         <v>2</v>
       </c>
-      <c r="K10" s="58"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>481</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>700</v>
+        <v>777</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="3" t="s">
-        <v>785</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>719</v>
+      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="58"/>
+      <c r="H11" s="58" t="s">
+        <v>747</v>
+      </c>
       <c r="I11" s="3" t="s">
-        <v>776</v>
+        <v>793</v>
       </c>
       <c r="J11" s="3">
-        <v>2</v>
-      </c>
-      <c r="K11" s="58"/>
+        <v>3</v>
+      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>486</v>
       </c>
@@ -9461,13 +9467,13 @@
           <x14:formula1>
             <xm:f>Configs!$O$3:$O$33</xm:f>
           </x14:formula1>
-          <xm:sqref>K3 K8:K11 K5 E8:E11 E2:E7</xm:sqref>
+          <xm:sqref>E2:E11 K2:K9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>HTS!$H$2:$H$25</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H7 B8:B11 B2:B7 H8:H11</xm:sqref>
+          <xm:sqref>B2:B11 H2:H11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fixed initial load of single options
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\livedev\apps\LiveHTS\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\palladium\source\cbs\LiveHTS\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6255,7 +6255,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:J6"/>
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6406,7 +6406,7 @@
         <v>671</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -6414,7 +6414,7 @@
         <v>605</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -6631,8 +6631,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
item _q template formatting.
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="19035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="19035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HTS Lab" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="744">
   <si>
     <t>Ever Tested?</t>
   </si>
@@ -2596,45 +2596,12 @@
     <t>KitName</t>
   </si>
   <si>
-    <t>K1</t>
-  </si>
-  <si>
-    <t>K2</t>
-  </si>
-  <si>
-    <t>Kit 1</t>
-  </si>
-  <si>
-    <t>Kit 2</t>
-  </si>
-  <si>
-    <t>K3</t>
-  </si>
-  <si>
-    <t>Kit 3</t>
-  </si>
-  <si>
     <t>KitName,  b25f9c72-852f-11e7-bb31-be2e44b06b34</t>
   </si>
   <si>
-    <t>K1,  b25f0456-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>K2,  b25f05aa-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>K3,  b25f0776-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>Ko</t>
-  </si>
-  <si>
     <t>Other Kit</t>
   </si>
   <si>
-    <t>Ko,  b25f0a50-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
     <t>HIV Test 1 Kit Name,  b26045aa-852f-11e7-bb31-be2e44b06b34</t>
   </si>
   <si>
@@ -2657,6 +2624,30 @@
   </si>
   <si>
     <t>I: Invalid,  b25f001e-852f-11e7-bb31-be2e44b06b34</t>
+  </si>
+  <si>
+    <t>Determine</t>
+  </si>
+  <si>
+    <t>First Response</t>
+  </si>
+  <si>
+    <t>KDT</t>
+  </si>
+  <si>
+    <t>KFR</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>KDT,  b25f0456-852f-11e7-bb31-be2e44b06b34</t>
+  </si>
+  <si>
+    <t>KFR,  b25f05aa-852f-11e7-bb31-be2e44b06b34</t>
+  </si>
+  <si>
+    <t>KO,  b25f0776-852f-11e7-bb31-be2e44b06b34</t>
   </si>
 </sst>
 </file>
@@ -4477,8 +4468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5197,7 +5188,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="E13" s="7" t="str">
         <f t="shared" ref="E13:E22" si="3">B13&amp;",  "&amp;A13</f>
@@ -5775,7 +5766,7 @@
         <v>635</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>746</v>
+        <v>735</v>
       </c>
       <c r="Q27" s="1">
         <v>3</v>
@@ -5844,14 +5835,14 @@
         <v>99</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>726</v>
+        <v>738</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="V29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>K1,  b25f0456-852f-11e7-bb31-be2e44b06b34</v>
+        <v>KDT,  b25f0456-852f-11e7-bb31-be2e44b06b34</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -5874,14 +5865,14 @@
         <v>100</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
       <c r="V30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>K2,  b25f05aa-852f-11e7-bb31-be2e44b06b34</v>
+        <v>KFR,  b25f05aa-852f-11e7-bb31-be2e44b06b34</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -5904,14 +5895,14 @@
         <v>101</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>730</v>
+        <v>740</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="V31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>K3,  b25f0776-852f-11e7-bb31-be2e44b06b34</v>
+        <v>KO,  b25f0776-852f-11e7-bb31-be2e44b06b34</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -5933,16 +5924,7 @@
       <c r="S32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="V32" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Ko,  b25f0a50-852f-11e7-bb31-be2e44b06b34</v>
-      </c>
+      <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -5973,10 +5955,10 @@
         <v>144</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
@@ -5994,10 +5976,10 @@
         <v>145</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="Q35" s="1">
         <v>2</v>
@@ -6015,10 +5997,10 @@
         <v>146</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
       <c r="Q36" s="1">
         <v>3</v>
@@ -6035,12 +6017,7 @@
       <c r="M37" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="N37" s="12" t="s">
-        <v>732</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>738</v>
-      </c>
+      <c r="N37" s="12"/>
       <c r="Q37" s="1">
         <v>4</v>
       </c>
@@ -6254,7 +6231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
@@ -6922,13 +6899,13 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6947,13 +6924,13 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6972,13 +6949,13 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>741</v>
+        <v>730</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>741</v>
+        <v>730</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -7022,13 +6999,13 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>742</v>
+        <v>731</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>742</v>
+        <v>731</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7047,13 +7024,13 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7072,13 +7049,13 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -7097,13 +7074,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added testing view model with multiple test results
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="19035" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="18195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HTS Lab" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="741">
   <si>
     <t>Ever Tested?</t>
   </si>
@@ -1299,18 +1299,6 @@
   </si>
   <si>
     <t>b262f386-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>b262f4ee-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>b262faac-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>b262fc32-852f-11e7-bb31-be2e44b06b34</t>
-  </si>
-  <si>
-    <t>b262fda4-852f-11e7-bb31-be2e44b06b34</t>
   </si>
   <si>
     <t>b262ff02-852f-11e7-bb31-be2e44b06b34</t>
@@ -2649,12 +2637,15 @@
   <si>
     <t>KO,  b25f0776-852f-11e7-bb31-be2e44b06b34</t>
   </si>
+  <si>
+    <t>HIV Test Form</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2717,6 +2708,14 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2744,7 +2743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2791,13 +2790,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2836,6 +2850,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3634,7 +3649,7 @@
         <v>233</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
@@ -3649,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H2" s="1" t="str">
         <f>D2&amp;",  "&amp;A2</f>
@@ -3661,7 +3676,7 @@
         <v>234</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
@@ -3676,7 +3691,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H3" s="1" t="str">
         <f t="shared" ref="H3:H24" si="0">D3&amp;",  "&amp;A3</f>
@@ -3688,7 +3703,7 @@
         <v>235</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
@@ -3703,7 +3718,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3715,7 +3730,7 @@
         <v>236</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C5" s="8">
         <v>4</v>
@@ -3730,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3742,7 +3757,7 @@
         <v>237</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C6" s="8">
         <v>5</v>
@@ -3757,7 +3772,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3769,7 +3784,7 @@
         <v>238</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C7" s="8">
         <v>6</v>
@@ -3784,7 +3799,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3796,22 +3811,22 @@
         <v>239</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C8" s="8">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="F8" s="1">
         <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3823,22 +3838,22 @@
         <v>240</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C9" s="8">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="F9" s="1">
         <v>9</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3850,22 +3865,22 @@
         <v>241</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C10" s="8">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="F10" s="1">
         <v>10</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3877,22 +3892,22 @@
         <v>242</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C11" s="8">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="F11" s="1">
         <v>11</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3904,22 +3919,22 @@
         <v>243</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C12" s="8">
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F12" s="1">
         <v>13</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3931,22 +3946,22 @@
         <v>244</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C13" s="8">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="F13" s="1">
         <v>14</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3958,22 +3973,22 @@
         <v>245</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C14" s="8">
         <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="F14" s="1">
         <v>15</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3985,22 +4000,22 @@
         <v>246</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C15" s="8">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F15" s="1">
         <v>16</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4012,7 +4027,7 @@
         <v>247</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C16" s="8">
         <v>17</v>
@@ -4027,7 +4042,7 @@
         <v>17</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4039,7 +4054,7 @@
         <v>248</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C17" s="8">
         <v>18</v>
@@ -4054,7 +4069,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4066,22 +4081,22 @@
         <v>255</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F18" s="1">
         <v>18.100000000000001</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H18" s="1" t="str">
         <f t="shared" ref="H18" si="1">D18&amp;",  "&amp;A18</f>
@@ -4093,7 +4108,7 @@
         <v>249</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C19" s="8">
         <v>19</v>
@@ -4108,7 +4123,7 @@
         <v>19</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4120,7 +4135,7 @@
         <v>250</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C20" s="8">
         <v>20</v>
@@ -4135,7 +4150,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4147,7 +4162,7 @@
         <v>251</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C21" s="8">
         <v>21</v>
@@ -4162,7 +4177,7 @@
         <v>21</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4174,7 +4189,7 @@
         <v>252</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C22" s="8">
         <v>22</v>
@@ -4189,7 +4204,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4201,7 +4216,7 @@
         <v>253</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C23" s="8">
         <v>23</v>
@@ -4216,7 +4231,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4228,7 +4243,7 @@
         <v>254</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C24" s="8">
         <v>24</v>
@@ -4243,7 +4258,7 @@
         <v>24</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4468,8 +4483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4520,7 +4535,7 @@
       </c>
       <c r="J1" s="13"/>
       <c r="M1" s="13" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
@@ -4538,7 +4553,7 @@
       </c>
       <c r="Y1" s="14"/>
       <c r="AB1" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -4611,7 +4626,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E3" s="7" t="str">
         <f t="shared" ref="E3:E12" si="0">B3&amp;",  "&amp;A3</f>
@@ -4634,10 +4649,10 @@
         <v>113</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
@@ -4669,7 +4684,7 @@
         <v>291</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -4703,10 +4718,10 @@
         <v>114</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="Q4" s="1">
         <v>2</v>
@@ -4746,7 +4761,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -4769,10 +4784,10 @@
         <v>115</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -4784,14 +4799,21 @@
         <v>18</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="V5" s="1" t="str">
-        <f t="shared" ref="V5:V32" si="2">T5&amp;",  "&amp;S5</f>
+        <f t="shared" ref="V5:V31" si="2">T5&amp;",  "&amp;S5</f>
         <v>NA,  b25ed1c0-852f-11e7-bb31-be2e44b06b34</v>
       </c>
       <c r="X5" s="7" t="s">
         <v>69</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="Z5" s="1" t="str">
+        <f>Y5&amp;",  "&amp;X5</f>
+        <v>HIV Test Form,  b25ec568-852f-11e7-bb31-be2e44b06b34</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -4805,7 +4827,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -4828,10 +4850,10 @@
         <v>116</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="Q6" s="1">
         <v>2</v>
@@ -4843,7 +4865,7 @@
         <v>17</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="V6" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4864,14 +4886,14 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Client tested as,  b25fbcca-852f-11e7-bb31-be2e44b06b34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>157</v>
@@ -4887,10 +4909,10 @@
         <v>117</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="Q7" s="1">
         <v>3</v>
@@ -4902,7 +4924,7 @@
         <v>21</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="V7" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4911,8 +4933,11 @@
       <c r="X7" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB7" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>178</v>
       </c>
@@ -4923,7 +4948,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -4933,7 +4958,7 @@
         <v>158</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
@@ -4943,10 +4968,10 @@
         <v>118</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="Q8" s="1">
         <v>4</v>
@@ -4958,7 +4983,7 @@
         <v>22</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="V8" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4967,6 +4992,12 @@
       <c r="X8" s="7" t="s">
         <v>72</v>
       </c>
+      <c r="AB8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC8" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -4979,7 +5010,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="0"/>
@@ -4989,7 +5020,7 @@
         <v>159</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
@@ -4999,10 +5030,10 @@
         <v>119</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="Q9" s="1">
         <v>5</v>
@@ -5014,7 +5045,7 @@
         <v>23</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="V9" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5032,7 +5063,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5042,7 +5073,7 @@
         <v>160</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="K10" s="7" t="str">
         <f t="shared" si="1"/>
@@ -5052,10 +5083,10 @@
         <v>120</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="Q10" s="1">
         <v>6</v>
@@ -5067,7 +5098,7 @@
         <v>24</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="V10" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5092,7 +5123,7 @@
         <v>161</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
@@ -5102,10 +5133,10 @@
         <v>121</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="Q11" s="1">
         <v>1</v>
@@ -5117,7 +5148,7 @@
         <v>45</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="V11" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5129,13 +5160,13 @@
         <v>182</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5145,7 +5176,7 @@
         <v>162</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
@@ -5155,10 +5186,10 @@
         <v>122</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="Q12" s="1">
         <v>2</v>
@@ -5170,7 +5201,7 @@
         <v>46</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="V12" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5182,13 +5213,13 @@
         <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="E13" s="7" t="str">
         <f t="shared" ref="E13:E22" si="3">B13&amp;",  "&amp;A13</f>
@@ -5202,10 +5233,10 @@
         <v>123</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="Q13" s="1">
         <v>1</v>
@@ -5217,7 +5248,7 @@
         <v>47</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="V13" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5229,7 +5260,7 @@
         <v>184</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -5246,10 +5277,10 @@
         <v>124</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="Q14" s="1">
         <v>2</v>
@@ -5261,7 +5292,7 @@
         <v>48</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="V14" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5273,10 +5304,10 @@
         <v>185</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E15" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5290,10 +5321,10 @@
         <v>125</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="Q15" s="1">
         <v>3</v>
@@ -5305,7 +5336,7 @@
         <v>49</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="V15" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5317,13 +5348,13 @@
         <v>186</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="E16" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5337,10 +5368,10 @@
         <v>126</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="Q16" s="1">
         <v>4</v>
@@ -5352,7 +5383,7 @@
         <v>50</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="V16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5370,7 +5401,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E17" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5384,10 +5415,10 @@
         <v>127</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="Q17" s="1">
         <v>5</v>
@@ -5399,7 +5430,7 @@
         <v>51</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="V17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5417,7 +5448,7 @@
         <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E18" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5431,10 +5462,10 @@
         <v>128</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="Q18" s="1">
         <v>6</v>
@@ -5446,7 +5477,7 @@
         <v>52</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="V18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5464,7 +5495,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="E19" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5478,10 +5509,10 @@
         <v>129</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="Q19" s="1">
         <v>1</v>
@@ -5493,7 +5524,7 @@
         <v>53</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="V19" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5511,7 +5542,7 @@
         <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E20" s="7" t="str">
         <f t="shared" si="3"/>
@@ -5525,10 +5556,10 @@
         <v>130</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="Q20" s="1">
         <v>2</v>
@@ -5540,7 +5571,7 @@
         <v>54</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="V20" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5552,7 +5583,7 @@
         <v>191</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>31</v>
@@ -5569,10 +5600,10 @@
         <v>131</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="Q21" s="1">
         <v>3</v>
@@ -5584,7 +5615,7 @@
         <v>55</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="V21" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5596,7 +5627,7 @@
         <v>192</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>31</v>
@@ -5613,10 +5644,10 @@
         <v>132</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="Q22" s="1">
         <v>4</v>
@@ -5628,7 +5659,7 @@
         <v>56</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="V22" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5643,10 +5674,10 @@
         <v>133</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Q23" s="1">
         <v>1</v>
@@ -5655,7 +5686,7 @@
         <v>93</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>7</v>
@@ -5673,10 +5704,10 @@
         <v>134</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="Q24" s="1">
         <v>2</v>
@@ -5685,7 +5716,7 @@
         <v>94</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>8</v>
@@ -5703,10 +5734,10 @@
         <v>135</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="Q25" s="1">
         <v>1</v>
@@ -5718,7 +5749,7 @@
         <v>20</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="V25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5733,10 +5764,10 @@
         <v>136</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="Q26" s="1">
         <v>2</v>
@@ -5748,7 +5779,7 @@
         <v>23</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="V26" s="1" t="str">
         <f>U26&amp;",  "&amp;S26</f>
@@ -5763,10 +5794,10 @@
         <v>137</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="Q27" s="1">
         <v>3</v>
@@ -5778,7 +5809,7 @@
         <v>45</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="V27" s="1" t="str">
         <f>U27&amp;",  "&amp;S27</f>
@@ -5793,10 +5824,10 @@
         <v>138</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="Q28" s="1">
         <v>1</v>
@@ -5805,10 +5836,10 @@
         <v>98</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="V28" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5823,10 +5854,10 @@
         <v>139</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="Q29" s="1">
         <v>2</v>
@@ -5835,10 +5866,10 @@
         <v>99</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="V29" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5853,10 +5884,10 @@
         <v>140</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="Q30" s="1">
         <v>3</v>
@@ -5865,10 +5896,10 @@
         <v>100</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="V30" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5883,10 +5914,10 @@
         <v>141</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="Q31" s="1">
         <v>1</v>
@@ -5895,10 +5926,10 @@
         <v>101</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="V31" s="1" t="str">
         <f t="shared" si="2"/>
@@ -5913,10 +5944,10 @@
         <v>142</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="Q32" s="1">
         <v>2</v>
@@ -5934,10 +5965,10 @@
         <v>143</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="Q33" s="1">
         <v>3</v>
@@ -5955,10 +5986,10 @@
         <v>144</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
@@ -5976,10 +6007,10 @@
         <v>145</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="Q35" s="1">
         <v>2</v>
@@ -5997,10 +6028,10 @@
         <v>146</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="Q36" s="1">
         <v>3</v>
@@ -6254,34 +6285,34 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>669</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6289,22 +6320,22 @@
         <v>352</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
@@ -6315,25 +6346,25 @@
         <v>353</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -6344,25 +6375,25 @@
         <v>354</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -6373,25 +6404,25 @@
         <v>355</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -6402,25 +6433,25 @@
         <v>356</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -6666,7 +6697,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -6678,10 +6709,10 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="L1" s="9" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -6689,25 +6720,25 @@
         <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>614</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>32</v>
@@ -6721,10 +6752,10 @@
         <v>292</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -6732,20 +6763,20 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6753,10 +6784,10 @@
         <v>293</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -6764,20 +6795,20 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -6785,10 +6816,10 @@
         <v>294</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -6796,13 +6827,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
@@ -6813,10 +6844,10 @@
         <v>295</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -6824,13 +6855,13 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -6838,10 +6869,10 @@
         <v>296</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -6849,13 +6880,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -6863,10 +6894,10 @@
         <v>297</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -6874,13 +6905,13 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -6888,10 +6919,10 @@
         <v>298</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -6899,13 +6930,13 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6913,10 +6944,10 @@
         <v>299</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -6924,13 +6955,13 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6938,10 +6969,10 @@
         <v>300</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -6949,13 +6980,13 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6963,10 +6994,10 @@
         <v>301</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -6974,13 +7005,13 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6988,10 +7019,10 @@
         <v>302</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -6999,13 +7030,13 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7013,10 +7044,10 @@
         <v>303</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -7024,13 +7055,13 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7038,10 +7069,10 @@
         <v>304</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -7049,13 +7080,13 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -7063,10 +7094,10 @@
         <v>305</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -7074,13 +7105,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7088,10 +7119,10 @@
         <v>306</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -7099,13 +7130,13 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -7113,10 +7144,10 @@
         <v>307</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -7124,13 +7155,13 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -7138,10 +7169,10 @@
         <v>308</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -7149,13 +7180,13 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7163,10 +7194,10 @@
         <v>309</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -7174,13 +7205,13 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -7188,10 +7219,10 @@
         <v>310</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -7199,13 +7230,13 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -7213,10 +7244,10 @@
         <v>311</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -7224,13 +7255,13 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -7238,10 +7269,10 @@
         <v>312</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -7249,13 +7280,13 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7263,10 +7294,10 @@
         <v>313</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -7274,13 +7305,13 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7288,10 +7319,10 @@
         <v>314</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -7299,13 +7330,13 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -7313,7 +7344,7 @@
         <v>315</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>29</v>
@@ -7326,7 +7357,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -7592,37 +7623,37 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>668</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>58</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7630,28 +7661,28 @@
         <v>392</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -7662,25 +7693,25 @@
         <v>393</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
@@ -7691,22 +7722,22 @@
         <v>394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="J4" s="1">
         <v>4</v>
@@ -7721,22 +7752,22 @@
         <v>395</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="J5" s="1">
         <v>5</v>
@@ -7752,28 +7783,28 @@
         <v>396</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="J6" s="1">
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
@@ -7784,22 +7815,22 @@
         <v>397</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -7814,22 +7845,22 @@
         <v>398</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="J8" s="1">
         <v>3</v>
@@ -7844,30 +7875,30 @@
         <v>399</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -7878,24 +7909,24 @@
         <v>400</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="J10" s="1">
         <v>2</v>
@@ -7910,24 +7941,24 @@
         <v>401</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="J11" s="1">
         <v>3</v>
@@ -8049,43 +8080,43 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>668</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8093,23 +8124,23 @@
         <v>412</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -8126,23 +8157,23 @@
         <v>413</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -8159,23 +8190,23 @@
         <v>414</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="J4" s="1">
         <v>2.1</v>
@@ -8192,35 +8223,35 @@
         <v>415</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="J5" s="1">
         <v>2.1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
@@ -8231,23 +8262,23 @@
         <v>416</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="J6" s="1">
         <v>2.2000000000000002</v>
@@ -8264,35 +8295,35 @@
         <v>417</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="J7" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
@@ -8356,10 +8387,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A142"/>
+  <dimension ref="A5:A142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8367,717 +8398,698 @@
     <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>426</v>
-      </c>
-    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed trace template stuff
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -4597,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView tabSelected="1" topLeftCell="L18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed opening of encounters
</commit_message>
<xml_diff>
--- a/Template/LiveHTS.xlsx
+++ b/Template/LiveHTS.xlsx
@@ -4597,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:Q40"/>
+    <sheetView tabSelected="1" topLeftCell="O18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>